<commit_message>
Added warrant rule to FTA batch template.
</commit_message>
<xml_diff>
--- a/db/Batch_FTA_Arraignments.xlsx
+++ b/db/Batch_FTA_Arraignments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\AppData\Local\Programs\Python\Python310\MuniEntry\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AABA9C9-A286-4DC1-84D3-BE3F35EC674C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF455577-AB0D-4C7E-BAE9-1DAA1903767A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45924" yWindow="6948" windowWidth="23352" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45972" yWindow="6996" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MuniEntryPleas" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
   <si>
     <t>17TRD22590</t>
   </si>
@@ -161,6 +161,18 @@
   </si>
   <si>
     <t>CaseEventDate</t>
+  </si>
+  <si>
+    <t>CaseTypeCode</t>
+  </si>
+  <si>
+    <t>TRD</t>
+  </si>
+  <si>
+    <t>TRC</t>
+  </si>
+  <si>
+    <t>CRB</t>
   </si>
 </sst>
 </file>
@@ -634,20 +646,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="13.73046875" customWidth="1"/>
     <col min="2" max="2" width="14.53125" customWidth="1"/>
-    <col min="3" max="5" width="13.73046875" customWidth="1"/>
+    <col min="3" max="6" width="13.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25.5">
+    <row r="1" spans="1:6" ht="25.5">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
@@ -658,13 +670,16 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -674,14 +689,17 @@
       <c r="C2" s="2">
         <v>44757</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -691,14 +709,17 @@
       <c r="C3" s="2">
         <v>44757</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -708,14 +729,17 @@
       <c r="C4" s="2">
         <v>44757</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -725,14 +749,17 @@
       <c r="C5" s="2">
         <v>44757</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -742,14 +769,17 @@
       <c r="C6" s="2">
         <v>44757</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -759,14 +789,17 @@
       <c r="C7" s="2">
         <v>44757</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -776,14 +809,17 @@
       <c r="C8" s="2">
         <v>44757</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -793,14 +829,17 @@
       <c r="C9" s="2">
         <v>44755</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
@@ -810,14 +849,17 @@
       <c r="C10" s="2">
         <v>44755</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -827,14 +869,17 @@
       <c r="C11" s="2">
         <v>44753</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
@@ -844,10 +889,13 @@
       <c r="C12" s="2">
         <v>44753</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>